<commit_message>
creatin SIS, added missing limit hi lo etc
</commit_message>
<xml_diff>
--- a/Element_list_export.xlsx
+++ b/Element_list_export.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P168"/>
+  <dimension ref="A1:P165"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="inlineStr"/>
@@ -1779,7 +1779,11 @@
           <t>1.410</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr"/>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Automatic Mousehole</t>
+        </is>
+      </c>
       <c r="F33" t="inlineStr"/>
       <c r="G33" t="inlineStr"/>
       <c r="H33" t="inlineStr"/>
@@ -1942,8 +1946,14 @@
       <c r="G37" t="n">
         <v>7</v>
       </c>
-      <c r="H37" t="inlineStr"/>
-      <c r="I37" t="inlineStr"/>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>S_LIMIT_HI_LO</t>
+        </is>
+      </c>
+      <c r="I37" t="n">
+        <v>6</v>
+      </c>
       <c r="J37" t="inlineStr"/>
       <c r="K37" t="inlineStr"/>
       <c r="L37" t="inlineStr"/>
@@ -1982,8 +1992,14 @@
       <c r="G38" t="n">
         <v>8</v>
       </c>
-      <c r="H38" t="inlineStr"/>
-      <c r="I38" t="inlineStr"/>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>S_LIMIT_HI_LO</t>
+        </is>
+      </c>
+      <c r="I38" t="n">
+        <v>7</v>
+      </c>
       <c r="J38" t="inlineStr"/>
       <c r="K38" t="inlineStr"/>
       <c r="L38" t="inlineStr"/>
@@ -2020,7 +2036,7 @@
         </is>
       </c>
       <c r="G39" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H39" t="inlineStr"/>
       <c r="I39" t="inlineStr"/>
@@ -2062,8 +2078,14 @@
       <c r="G40" t="n">
         <v>9</v>
       </c>
-      <c r="H40" t="inlineStr"/>
-      <c r="I40" t="inlineStr"/>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>S_LIMIT_HI_LO</t>
+        </is>
+      </c>
+      <c r="I40" t="n">
+        <v>9</v>
+      </c>
       <c r="J40" t="inlineStr"/>
       <c r="K40" t="inlineStr"/>
       <c r="L40" t="inlineStr"/>
@@ -2100,7 +2122,7 @@
         </is>
       </c>
       <c r="G41" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H41" t="inlineStr"/>
       <c r="I41" t="inlineStr"/>
@@ -2236,7 +2258,7 @@
         </is>
       </c>
       <c r="K44" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="L44" t="inlineStr"/>
       <c r="M44" t="inlineStr"/>
@@ -2288,7 +2310,7 @@
         </is>
       </c>
       <c r="K45" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="L45" t="inlineStr"/>
       <c r="M45" t="inlineStr"/>
@@ -2324,7 +2346,7 @@
         </is>
       </c>
       <c r="G46" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H46" t="inlineStr"/>
       <c r="I46" t="inlineStr"/>
@@ -2371,10 +2393,8 @@
           <t>S_LIMIT_HI_LO</t>
         </is>
       </c>
-      <c r="I47" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
+      <c r="I47" t="n">
+        <v>16</v>
       </c>
       <c r="J47" t="inlineStr"/>
       <c r="K47" t="inlineStr"/>
@@ -2408,7 +2428,7 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>S_SIS</t>
+          <t>S_PUMP_TEST</t>
         </is>
       </c>
       <c r="G48" t="n">
@@ -2416,16 +2436,30 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>A_PUMPS</t>
+          <t>S_SIS</t>
         </is>
       </c>
       <c r="I48" t="n">
         <v>1</v>
       </c>
-      <c r="J48" t="inlineStr"/>
-      <c r="K48" t="inlineStr"/>
-      <c r="L48" t="inlineStr"/>
-      <c r="M48" t="inlineStr"/>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>pump_nr</t>
+        </is>
+      </c>
+      <c r="K48" t="n">
+        <v>1</v>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>Pump[x]</t>
+        </is>
+      </c>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="N48" t="inlineStr"/>
       <c r="O48" t="inlineStr"/>
       <c r="P48" t="inlineStr"/>
@@ -2578,7 +2612,7 @@
         </is>
       </c>
       <c r="G52" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H52" t="inlineStr"/>
       <c r="I52" t="inlineStr"/>
@@ -2614,7 +2648,7 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>S_SIS</t>
+          <t>S_PUMP_TEST</t>
         </is>
       </c>
       <c r="G53" t="n">
@@ -2622,16 +2656,30 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>A_PUMPS</t>
+          <t>S_SIS</t>
         </is>
       </c>
       <c r="I53" t="n">
+        <v>1</v>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>pump_nr</t>
+        </is>
+      </c>
+      <c r="K53" t="n">
         <v>2</v>
       </c>
-      <c r="J53" t="inlineStr"/>
-      <c r="K53" t="inlineStr"/>
-      <c r="L53" t="inlineStr"/>
-      <c r="M53" t="inlineStr"/>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>Pump[x]</t>
+        </is>
+      </c>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="N53" t="inlineStr"/>
       <c r="O53" t="inlineStr"/>
       <c r="P53" t="inlineStr"/>
@@ -2784,7 +2832,7 @@
         </is>
       </c>
       <c r="G57" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H57" t="inlineStr"/>
       <c r="I57" t="inlineStr"/>
@@ -2820,7 +2868,7 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>S_SIS</t>
+          <t>S_PUMP_TEST</t>
         </is>
       </c>
       <c r="G58" t="n">
@@ -2828,16 +2876,30 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>A_PUMPS</t>
+          <t>S_SIS</t>
         </is>
       </c>
       <c r="I58" t="n">
+        <v>1</v>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>pump_nr</t>
+        </is>
+      </c>
+      <c r="K58" t="n">
         <v>3</v>
       </c>
-      <c r="J58" t="inlineStr"/>
-      <c r="K58" t="inlineStr"/>
-      <c r="L58" t="inlineStr"/>
-      <c r="M58" t="inlineStr"/>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>Pump[x]</t>
+        </is>
+      </c>
+      <c r="M58" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="N58" t="inlineStr"/>
       <c r="O58" t="inlineStr"/>
       <c r="P58" t="inlineStr"/>
@@ -2990,7 +3052,7 @@
         </is>
       </c>
       <c r="G62" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H62" t="inlineStr"/>
       <c r="I62" t="inlineStr"/>
@@ -3070,7 +3132,7 @@
         </is>
       </c>
       <c r="G64" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H64" t="inlineStr"/>
       <c r="I64" t="inlineStr"/>
@@ -3110,7 +3172,7 @@
         </is>
       </c>
       <c r="G65" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H65" t="inlineStr"/>
       <c r="I65" t="inlineStr"/>
@@ -3166,7 +3228,7 @@
         </is>
       </c>
       <c r="K66" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L66" t="inlineStr"/>
       <c r="M66" t="inlineStr"/>
@@ -3218,7 +3280,7 @@
         </is>
       </c>
       <c r="K67" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="L67" t="inlineStr"/>
       <c r="M67" t="inlineStr"/>
@@ -3254,7 +3316,7 @@
         </is>
       </c>
       <c r="G68" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H68" t="inlineStr"/>
       <c r="I68" t="inlineStr"/>
@@ -3310,7 +3372,7 @@
         </is>
       </c>
       <c r="K69" t="n">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="L69" t="inlineStr"/>
       <c r="M69" t="inlineStr"/>
@@ -3346,7 +3408,7 @@
         </is>
       </c>
       <c r="G70" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="H70" t="inlineStr"/>
       <c r="I70" t="inlineStr"/>
@@ -3426,7 +3488,7 @@
         </is>
       </c>
       <c r="G72" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="H72" t="inlineStr"/>
       <c r="I72" t="inlineStr"/>
@@ -3466,7 +3528,7 @@
         </is>
       </c>
       <c r="G73" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H73" t="inlineStr"/>
       <c r="I73" t="inlineStr"/>
@@ -3506,7 +3568,7 @@
         </is>
       </c>
       <c r="G74" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="H74" t="inlineStr"/>
       <c r="I74" t="inlineStr"/>
@@ -3546,7 +3608,7 @@
         </is>
       </c>
       <c r="G75" t="n">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="H75" t="inlineStr"/>
       <c r="I75" t="inlineStr"/>
@@ -3586,7 +3648,7 @@
         </is>
       </c>
       <c r="G76" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H76" t="inlineStr"/>
       <c r="I76" t="inlineStr"/>
@@ -3673,10 +3735,8 @@
           <t>S_LIMIT_HI_LO</t>
         </is>
       </c>
-      <c r="I78" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
+      <c r="I78" t="n">
+        <v>26</v>
       </c>
       <c r="J78" t="inlineStr"/>
       <c r="K78" t="inlineStr"/>
@@ -3762,7 +3822,7 @@
         </is>
       </c>
       <c r="I80" t="n">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="J80" t="inlineStr"/>
       <c r="K80" t="inlineStr"/>
@@ -3808,7 +3868,7 @@
         </is>
       </c>
       <c r="I81" t="n">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="J81" t="inlineStr"/>
       <c r="K81" t="inlineStr"/>
@@ -3854,7 +3914,7 @@
         </is>
       </c>
       <c r="I82" t="n">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="J82" t="inlineStr"/>
       <c r="K82" t="inlineStr"/>
@@ -3900,7 +3960,7 @@
         </is>
       </c>
       <c r="I83" t="n">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="J83" t="inlineStr"/>
       <c r="K83" t="inlineStr"/>
@@ -3946,7 +4006,7 @@
         </is>
       </c>
       <c r="I84" t="n">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="J84" t="inlineStr"/>
       <c r="K84" t="inlineStr"/>
@@ -3992,7 +4052,7 @@
         </is>
       </c>
       <c r="I85" t="n">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="J85" t="inlineStr"/>
       <c r="K85" t="inlineStr"/>
@@ -5578,7 +5638,7 @@
         </is>
       </c>
       <c r="G119" t="n">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H119" t="inlineStr"/>
       <c r="I119" t="inlineStr"/>
@@ -5658,7 +5718,7 @@
         </is>
       </c>
       <c r="G121" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="H121" t="inlineStr"/>
       <c r="I121" t="inlineStr"/>
@@ -5854,7 +5914,7 @@
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>S_SIS</t>
+          <t>S_PUMP_TEST</t>
         </is>
       </c>
       <c r="G126" t="n">
@@ -5862,16 +5922,30 @@
       </c>
       <c r="H126" t="inlineStr">
         <is>
-          <t>A_PUMPS</t>
+          <t>S_SIS</t>
         </is>
       </c>
       <c r="I126" t="n">
+        <v>2</v>
+      </c>
+      <c r="J126" t="inlineStr">
+        <is>
+          <t>pump_nr</t>
+        </is>
+      </c>
+      <c r="K126" t="n">
         <v>4</v>
       </c>
-      <c r="J126" t="inlineStr"/>
-      <c r="K126" t="inlineStr"/>
-      <c r="L126" t="inlineStr"/>
-      <c r="M126" t="inlineStr"/>
+      <c r="L126" t="inlineStr">
+        <is>
+          <t>Pump[x]</t>
+        </is>
+      </c>
+      <c r="M126" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="N126" t="inlineStr"/>
       <c r="O126" t="inlineStr"/>
       <c r="P126" t="inlineStr"/>
@@ -6024,7 +6098,7 @@
         </is>
       </c>
       <c r="G130" t="n">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H130" t="inlineStr"/>
       <c r="I130" t="inlineStr"/>
@@ -6060,7 +6134,7 @@
       </c>
       <c r="F131" t="inlineStr">
         <is>
-          <t>S_SIS</t>
+          <t>S_PUMP_TEST</t>
         </is>
       </c>
       <c r="G131" t="n">
@@ -6068,16 +6142,30 @@
       </c>
       <c r="H131" t="inlineStr">
         <is>
-          <t>A_PUMPS</t>
+          <t>S_SIS</t>
         </is>
       </c>
       <c r="I131" t="n">
+        <v>2</v>
+      </c>
+      <c r="J131" t="inlineStr">
+        <is>
+          <t>pump_nr</t>
+        </is>
+      </c>
+      <c r="K131" t="n">
         <v>5</v>
       </c>
-      <c r="J131" t="inlineStr"/>
-      <c r="K131" t="inlineStr"/>
-      <c r="L131" t="inlineStr"/>
-      <c r="M131" t="inlineStr"/>
+      <c r="L131" t="inlineStr">
+        <is>
+          <t>Pump[x]</t>
+        </is>
+      </c>
+      <c r="M131" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="N131" t="inlineStr"/>
       <c r="O131" t="inlineStr"/>
       <c r="P131" t="inlineStr"/>
@@ -6230,7 +6318,7 @@
         </is>
       </c>
       <c r="G135" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H135" t="inlineStr"/>
       <c r="I135" t="inlineStr"/>
@@ -6266,7 +6354,7 @@
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>S_SIS</t>
+          <t>S_PUMP_TEST</t>
         </is>
       </c>
       <c r="G136" t="n">
@@ -6274,16 +6362,30 @@
       </c>
       <c r="H136" t="inlineStr">
         <is>
-          <t>A_PUMPS</t>
+          <t>S_SIS</t>
         </is>
       </c>
       <c r="I136" t="n">
+        <v>2</v>
+      </c>
+      <c r="J136" t="inlineStr">
+        <is>
+          <t>pump_nr</t>
+        </is>
+      </c>
+      <c r="K136" t="n">
         <v>6</v>
       </c>
-      <c r="J136" t="inlineStr"/>
-      <c r="K136" t="inlineStr"/>
-      <c r="L136" t="inlineStr"/>
-      <c r="M136" t="inlineStr"/>
+      <c r="L136" t="inlineStr">
+        <is>
+          <t>Pump[x]</t>
+        </is>
+      </c>
+      <c r="M136" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="N136" t="inlineStr"/>
       <c r="O136" t="inlineStr"/>
       <c r="P136" t="inlineStr"/>
@@ -6396,7 +6498,7 @@
         </is>
       </c>
       <c r="G139" t="n">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="H139" t="inlineStr"/>
       <c r="I139" t="inlineStr"/>
@@ -6482,7 +6584,7 @@
         </is>
       </c>
       <c r="I141" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J141" t="inlineStr">
         <is>
@@ -6530,7 +6632,7 @@
         </is>
       </c>
       <c r="G142" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="H142" t="inlineStr"/>
       <c r="I142" t="inlineStr"/>
@@ -6568,7 +6670,7 @@
         </is>
       </c>
       <c r="G143" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H143" t="inlineStr"/>
       <c r="I143" t="inlineStr"/>
@@ -6606,7 +6708,7 @@
         </is>
       </c>
       <c r="G144" t="n">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="H144" t="inlineStr"/>
       <c r="I144" t="inlineStr"/>
@@ -6644,7 +6746,7 @@
         </is>
       </c>
       <c r="G145" t="n">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H145" t="inlineStr"/>
       <c r="I145" t="inlineStr"/>
@@ -6682,7 +6784,7 @@
         </is>
       </c>
       <c r="G146" t="n">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="H146" t="inlineStr"/>
       <c r="I146" t="inlineStr"/>
@@ -6720,7 +6822,7 @@
         </is>
       </c>
       <c r="G147" t="n">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="H147" t="inlineStr"/>
       <c r="I147" t="inlineStr"/>
@@ -6758,7 +6860,7 @@
         </is>
       </c>
       <c r="G148" t="n">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H148" t="inlineStr"/>
       <c r="I148" t="inlineStr"/>
@@ -6796,7 +6898,7 @@
         </is>
       </c>
       <c r="G149" t="n">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="H149" t="inlineStr"/>
       <c r="I149" t="inlineStr"/>
@@ -6834,7 +6936,7 @@
         </is>
       </c>
       <c r="G150" t="n">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="H150" t="inlineStr"/>
       <c r="I150" t="inlineStr"/>
@@ -6872,7 +6974,7 @@
         </is>
       </c>
       <c r="G151" t="n">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H151" t="inlineStr"/>
       <c r="I151" t="inlineStr"/>
@@ -6910,7 +7012,7 @@
         </is>
       </c>
       <c r="G152" t="n">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="H152" t="inlineStr">
         <is>
@@ -6954,7 +7056,7 @@
         </is>
       </c>
       <c r="G153" t="n">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="H153" t="inlineStr"/>
       <c r="I153" t="inlineStr"/>
@@ -6992,7 +7094,7 @@
         </is>
       </c>
       <c r="G154" t="n">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H154" t="inlineStr"/>
       <c r="I154" t="inlineStr"/>
@@ -7030,7 +7132,7 @@
         </is>
       </c>
       <c r="G155" t="n">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="H155" t="inlineStr"/>
       <c r="I155" t="inlineStr"/>
@@ -7068,7 +7170,7 @@
         </is>
       </c>
       <c r="G156" t="n">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H156" t="inlineStr"/>
       <c r="I156" t="inlineStr"/>
@@ -7085,59 +7187,41 @@
         <v>155</v>
       </c>
       <c r="B157" t="n">
-        <v>1.815</v>
+        <v>1.55</v>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>[SIS]</t>
+          <t>['GIA', 'K', 'Y', 'YC']</t>
         </is>
       </c>
       <c r="D157" t="inlineStr"/>
       <c r="E157" t="inlineStr">
         <is>
-          <t>SIS MODULE</t>
+          <t>Exhaust air flap</t>
         </is>
       </c>
       <c r="F157" t="inlineStr">
         <is>
-          <t>S_SIS</t>
+          <t>S_LIMIT_HI_LO</t>
         </is>
       </c>
       <c r="G157" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H157" t="inlineStr">
         <is>
-          <t>A_DOSING_UNIT</t>
+          <t>S_MOTOR1</t>
         </is>
       </c>
       <c r="I157" t="n">
-        <v>1</v>
-      </c>
-      <c r="J157" t="inlineStr">
-        <is>
-          <t>S_LIMIT_HI_LO</t>
-        </is>
-      </c>
-      <c r="K157" t="n">
-        <v>15</v>
-      </c>
-      <c r="L157" t="inlineStr">
-        <is>
-          <t>S_LIMIT_HI_LO</t>
-        </is>
-      </c>
-      <c r="M157" t="n">
-        <v>12</v>
-      </c>
-      <c r="N157" t="inlineStr">
-        <is>
-          <t>S_LIMIT_HI_LO</t>
-        </is>
-      </c>
-      <c r="O157" t="n">
-        <v>13</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="J157" t="inlineStr"/>
+      <c r="K157" t="inlineStr"/>
+      <c r="L157" t="inlineStr"/>
+      <c r="M157" t="inlineStr"/>
+      <c r="N157" t="inlineStr"/>
+      <c r="O157" t="inlineStr"/>
       <c r="P157" t="inlineStr"/>
     </row>
     <row r="158">
@@ -7145,34 +7229,34 @@
         <v>156</v>
       </c>
       <c r="B158" t="n">
-        <v>1.815</v>
+        <v>1.555</v>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>[PTEST]</t>
+          <t>['GIA', 'V', 'Y', 'YC']</t>
         </is>
       </c>
       <c r="D158" t="inlineStr"/>
       <c r="E158" t="inlineStr">
         <is>
-          <t>PUMP TEST MODULE</t>
+          <t>Exhaust bypass valve</t>
         </is>
       </c>
       <c r="F158" t="inlineStr">
         <is>
-          <t>S_PUMP_TEST</t>
+          <t>S_LIMIT_HI_LO</t>
         </is>
       </c>
       <c r="G158" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="H158" t="inlineStr">
         <is>
-          <t>A_DOSING_UNIT</t>
+          <t>S_MOTOR1</t>
         </is>
       </c>
       <c r="I158" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="J158" t="inlineStr"/>
       <c r="K158" t="inlineStr"/>
@@ -7187,51 +7271,39 @@
         <v>157</v>
       </c>
       <c r="B159" t="n">
-        <v>1.815</v>
+        <v>1.56</v>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>[DU]</t>
+          <t>['GIA', 'K', 'Y', 'YC']</t>
         </is>
       </c>
       <c r="D159" t="inlineStr"/>
       <c r="E159" t="inlineStr">
         <is>
-          <t>DOSING UNIT MODULE</t>
+          <t>Exhaust air flap</t>
         </is>
       </c>
       <c r="F159" t="inlineStr">
         <is>
-          <t>A_DOSING_UNIT</t>
+          <t>S_LIMIT_HI_LO</t>
         </is>
       </c>
       <c r="G159" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="H159" t="inlineStr">
         <is>
-          <t>S_WEIGHT_SCALE2_NG</t>
+          <t>S_MOTOR1</t>
         </is>
       </c>
       <c r="I159" t="n">
-        <v>1</v>
-      </c>
-      <c r="J159" t="inlineStr">
-        <is>
-          <t>S_SIS</t>
-        </is>
-      </c>
-      <c r="K159" t="n">
-        <v>1</v>
-      </c>
-      <c r="L159" t="inlineStr">
-        <is>
-          <t>S_PUMP_TEST</t>
-        </is>
-      </c>
-      <c r="M159" t="n">
-        <v>1</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="J159" t="inlineStr"/>
+      <c r="K159" t="inlineStr"/>
+      <c r="L159" t="inlineStr"/>
+      <c r="M159" t="inlineStr"/>
       <c r="N159" t="inlineStr"/>
       <c r="O159" t="inlineStr"/>
       <c r="P159" t="inlineStr"/>
@@ -7241,59 +7313,41 @@
         <v>158</v>
       </c>
       <c r="B160" t="n">
-        <v>1.816</v>
+        <v>1.865</v>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>[SIS]</t>
+          <t>['PSA-', 'V']</t>
         </is>
       </c>
       <c r="D160" t="inlineStr"/>
       <c r="E160" t="inlineStr">
         <is>
-          <t>SIS MODULE</t>
+          <t>Inflatable Gasket</t>
         </is>
       </c>
       <c r="F160" t="inlineStr">
         <is>
-          <t>S_SIS</t>
+          <t>S_LIMIT_HI_LO</t>
         </is>
       </c>
       <c r="G160" t="n">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="H160" t="inlineStr">
         <is>
-          <t>A_DOSING_UNIT</t>
+          <t>S_GASKET</t>
         </is>
       </c>
       <c r="I160" t="n">
-        <v>2</v>
-      </c>
-      <c r="J160" t="inlineStr">
-        <is>
-          <t>S_LIMIT_HI_LO</t>
-        </is>
-      </c>
-      <c r="K160" t="n">
-        <v>17</v>
-      </c>
-      <c r="L160" t="inlineStr">
-        <is>
-          <t>S_LIMIT_HI_LO</t>
-        </is>
-      </c>
-      <c r="M160" t="n">
-        <v>12</v>
-      </c>
-      <c r="N160" t="inlineStr">
-        <is>
-          <t>S_LIMIT_HI_LO</t>
-        </is>
-      </c>
-      <c r="O160" t="n">
-        <v>13</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="J160" t="inlineStr"/>
+      <c r="K160" t="inlineStr"/>
+      <c r="L160" t="inlineStr"/>
+      <c r="M160" t="inlineStr"/>
+      <c r="N160" t="inlineStr"/>
+      <c r="O160" t="inlineStr"/>
       <c r="P160" t="inlineStr"/>
     </row>
     <row r="161">
@@ -7301,30 +7355,30 @@
         <v>159</v>
       </c>
       <c r="B161" t="n">
-        <v>1.816</v>
+        <v>1.866</v>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>[PTEST]</t>
+          <t>['PSA-', 'V']</t>
         </is>
       </c>
       <c r="D161" t="inlineStr"/>
       <c r="E161" t="inlineStr">
         <is>
-          <t>PUMP TEST MODULE</t>
+          <t>Inflatable Gasket</t>
         </is>
       </c>
       <c r="F161" t="inlineStr">
         <is>
-          <t>S_PUMP_TEST</t>
+          <t>S_LIMIT_HI_LO</t>
         </is>
       </c>
       <c r="G161" t="n">
-        <v>2</v>
+        <v>49</v>
       </c>
       <c r="H161" t="inlineStr">
         <is>
-          <t>A_DOSING_UNIT</t>
+          <t>S_GASKET</t>
         </is>
       </c>
       <c r="I161" t="n">
@@ -7343,51 +7397,39 @@
         <v>160</v>
       </c>
       <c r="B162" t="n">
-        <v>1.816</v>
+        <v>1.867</v>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>[DU]</t>
+          <t>['PSA-', 'V']</t>
         </is>
       </c>
       <c r="D162" t="inlineStr"/>
       <c r="E162" t="inlineStr">
         <is>
-          <t>DOSING UNIT MODULE</t>
+          <t>Inflatable Gasket</t>
         </is>
       </c>
       <c r="F162" t="inlineStr">
         <is>
-          <t>A_DOSING_UNIT</t>
+          <t>S_LIMIT_HI_LO</t>
         </is>
       </c>
       <c r="G162" t="n">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="H162" t="inlineStr">
         <is>
-          <t>S_WEIGHT_SCALE2_NG</t>
+          <t>S_GASKET</t>
         </is>
       </c>
       <c r="I162" t="n">
-        <v>2</v>
-      </c>
-      <c r="J162" t="inlineStr">
-        <is>
-          <t>S_SIS</t>
-        </is>
-      </c>
-      <c r="K162" t="n">
-        <v>2</v>
-      </c>
-      <c r="L162" t="inlineStr">
-        <is>
-          <t>S_PUMP_TEST</t>
-        </is>
-      </c>
-      <c r="M162" t="n">
-        <v>2</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="J162" t="inlineStr"/>
+      <c r="K162" t="inlineStr"/>
+      <c r="L162" t="inlineStr"/>
+      <c r="M162" t="inlineStr"/>
       <c r="N162" t="inlineStr"/>
       <c r="O162" t="inlineStr"/>
       <c r="P162" t="inlineStr"/>
@@ -7397,7 +7439,7 @@
         <v>161</v>
       </c>
       <c r="B163" t="n">
-        <v>1.865</v>
+        <v>1.868</v>
       </c>
       <c r="C163" t="inlineStr">
         <is>
@@ -7416,7 +7458,7 @@
         </is>
       </c>
       <c r="G163" t="n">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="H163" t="inlineStr">
         <is>
@@ -7424,7 +7466,7 @@
         </is>
       </c>
       <c r="I163" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J163" t="inlineStr"/>
       <c r="K163" t="inlineStr"/>
@@ -7439,7 +7481,7 @@
         <v>162</v>
       </c>
       <c r="B164" t="n">
-        <v>1.866</v>
+        <v>1.869</v>
       </c>
       <c r="C164" t="inlineStr">
         <is>
@@ -7458,7 +7500,7 @@
         </is>
       </c>
       <c r="G164" t="n">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="H164" t="inlineStr">
         <is>
@@ -7466,7 +7508,7 @@
         </is>
       </c>
       <c r="I164" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J164" t="inlineStr"/>
       <c r="K164" t="inlineStr"/>
@@ -7481,7 +7523,7 @@
         <v>163</v>
       </c>
       <c r="B165" t="n">
-        <v>1.867</v>
+        <v>1.87</v>
       </c>
       <c r="C165" t="inlineStr">
         <is>
@@ -7500,7 +7542,7 @@
         </is>
       </c>
       <c r="G165" t="n">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="H165" t="inlineStr">
         <is>
@@ -7508,7 +7550,7 @@
         </is>
       </c>
       <c r="I165" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J165" t="inlineStr"/>
       <c r="K165" t="inlineStr"/>
@@ -7518,132 +7560,6 @@
       <c r="O165" t="inlineStr"/>
       <c r="P165" t="inlineStr"/>
     </row>
-    <row r="166">
-      <c r="A166" s="1" t="n">
-        <v>164</v>
-      </c>
-      <c r="B166" t="n">
-        <v>1.868</v>
-      </c>
-      <c r="C166" t="inlineStr">
-        <is>
-          <t>['PSA-', 'V']</t>
-        </is>
-      </c>
-      <c r="D166" t="inlineStr"/>
-      <c r="E166" t="inlineStr">
-        <is>
-          <t>Inflatable Gasket</t>
-        </is>
-      </c>
-      <c r="F166" t="inlineStr">
-        <is>
-          <t>S_LIMIT_HI_LO</t>
-        </is>
-      </c>
-      <c r="G166" t="n">
-        <v>48</v>
-      </c>
-      <c r="H166" t="inlineStr">
-        <is>
-          <t>S_GASKET</t>
-        </is>
-      </c>
-      <c r="I166" t="n">
-        <v>4</v>
-      </c>
-      <c r="J166" t="inlineStr"/>
-      <c r="K166" t="inlineStr"/>
-      <c r="L166" t="inlineStr"/>
-      <c r="M166" t="inlineStr"/>
-      <c r="N166" t="inlineStr"/>
-      <c r="O166" t="inlineStr"/>
-      <c r="P166" t="inlineStr"/>
-    </row>
-    <row r="167">
-      <c r="A167" s="1" t="n">
-        <v>165</v>
-      </c>
-      <c r="B167" t="n">
-        <v>1.869</v>
-      </c>
-      <c r="C167" t="inlineStr">
-        <is>
-          <t>['PSA-', 'V']</t>
-        </is>
-      </c>
-      <c r="D167" t="inlineStr"/>
-      <c r="E167" t="inlineStr">
-        <is>
-          <t>Inflatable Gasket</t>
-        </is>
-      </c>
-      <c r="F167" t="inlineStr">
-        <is>
-          <t>S_LIMIT_HI_LO</t>
-        </is>
-      </c>
-      <c r="G167" t="n">
-        <v>49</v>
-      </c>
-      <c r="H167" t="inlineStr">
-        <is>
-          <t>S_GASKET</t>
-        </is>
-      </c>
-      <c r="I167" t="n">
-        <v>5</v>
-      </c>
-      <c r="J167" t="inlineStr"/>
-      <c r="K167" t="inlineStr"/>
-      <c r="L167" t="inlineStr"/>
-      <c r="M167" t="inlineStr"/>
-      <c r="N167" t="inlineStr"/>
-      <c r="O167" t="inlineStr"/>
-      <c r="P167" t="inlineStr"/>
-    </row>
-    <row r="168">
-      <c r="A168" s="1" t="n">
-        <v>166</v>
-      </c>
-      <c r="B168" t="n">
-        <v>1.87</v>
-      </c>
-      <c r="C168" t="inlineStr">
-        <is>
-          <t>['PSA-', 'V']</t>
-        </is>
-      </c>
-      <c r="D168" t="inlineStr"/>
-      <c r="E168" t="inlineStr">
-        <is>
-          <t>Inflatable Gasket</t>
-        </is>
-      </c>
-      <c r="F168" t="inlineStr">
-        <is>
-          <t>S_LIMIT_HI_LO</t>
-        </is>
-      </c>
-      <c r="G168" t="n">
-        <v>50</v>
-      </c>
-      <c r="H168" t="inlineStr">
-        <is>
-          <t>S_GASKET</t>
-        </is>
-      </c>
-      <c r="I168" t="n">
-        <v>6</v>
-      </c>
-      <c r="J168" t="inlineStr"/>
-      <c r="K168" t="inlineStr"/>
-      <c r="L168" t="inlineStr"/>
-      <c r="M168" t="inlineStr"/>
-      <c r="N168" t="inlineStr"/>
-      <c r="O168" t="inlineStr"/>
-      <c r="P168" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>